<commit_message>
Auw_combine executed Production and development.
</commit_message>
<xml_diff>
--- a/AUW_Combine/Reports_Combine/Report details.xlsx
+++ b/AUW_Combine/Reports_Combine/Report details.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sweta\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +50,9 @@
   </si>
   <si>
     <t>Test cases iitially fail because of page load affected by network</t>
+  </si>
+  <si>
+    <t>Production</t>
   </si>
 </sst>
 </file>
@@ -408,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +470,46 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>44545</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>119</v>
+      </c>
+      <c r="D3" s="4">
+        <v>119</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44545</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>134</v>
+      </c>
+      <c r="D4" s="4">
+        <v>132</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AUW Combine executed and updated
</commit_message>
<xml_diff>
--- a/AUW_Combine/Reports_Combine/Report details.xlsx
+++ b/AUW_Combine/Reports_Combine/Report details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +510,52 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44546</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>119</v>
+      </c>
+      <c r="D5" s="4">
+        <v>118</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44545</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4">
+        <v>134</v>
+      </c>
+      <c r="D6" s="4">
+        <v>131</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AUW Combine Production is executed (Warranty is not added in production Script)
</commit_message>
<xml_diff>
--- a/AUW_Combine/Reports_Combine/Report details.xlsx
+++ b/AUW_Combine/Reports_Combine/Report details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Production</t>
+  </si>
+  <si>
+    <t>Test cases initially fail because of page load affected by network</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -126,6 +129,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +559,30 @@
         <v>8</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>44560</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
+        <v>134</v>
+      </c>
+      <c r="D7" s="4">
+        <v>133</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AUE combine executed on prod and development
</commit_message>
<xml_diff>
--- a/AUW_Combine/Reports_Combine/Report details.xlsx
+++ b/AUW_Combine/Reports_Combine/Report details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,6 +585,52 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44565</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>119</v>
+      </c>
+      <c r="D8" s="4">
+        <v>117</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>44565</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4">
+        <v>134</v>
+      </c>
+      <c r="D9" s="4">
+        <v>129</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AUW_combine executed and Updated
</commit_message>
<xml_diff>
--- a/AUW_Combine/Reports_Combine/Report details.xlsx
+++ b/AUW_Combine/Reports_Combine/Report details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +631,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>44566</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4">
+        <v>134</v>
+      </c>
+      <c r="D10" s="4">
+        <v>132</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>44566</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>119</v>
+      </c>
+      <c r="D11" s="4">
+        <v>119</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Executed on prod and dev
</commit_message>
<xml_diff>
--- a/AUW_Combine/Reports_Combine/Report details.xlsx
+++ b/AUW_Combine/Reports_Combine/Report details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12705" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11130" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -31,16 +31,10 @@
     <t>Development</t>
   </si>
   <si>
-    <t>Passtest case</t>
-  </si>
-  <si>
     <t>Fail cases</t>
   </si>
   <si>
     <t xml:space="preserve">Comments </t>
-  </si>
-  <si>
-    <t>Total Tcexecuted</t>
   </si>
   <si>
     <t xml:space="preserve">Result After analysing </t>
@@ -416,18 +410,16 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:L13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="21" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -438,19 +430,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -461,19 +447,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="4">
-        <v>120</v>
-      </c>
-      <c r="D2" s="4">
-        <v>116</v>
-      </c>
-      <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>9</v>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -484,12 +464,6 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>119</v>
-      </c>
-      <c r="D3" s="4">
-        <v>119</v>
-      </c>
-      <c r="E3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -498,22 +472,16 @@
         <v>44545</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4">
-        <v>134</v>
-      </c>
-      <c r="D4" s="4">
-        <v>132</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -524,19 +492,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>119</v>
-      </c>
-      <c r="D5" s="4">
-        <v>118</v>
-      </c>
-      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>9</v>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -544,22 +506,16 @@
         <v>44545</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>134</v>
-      </c>
-      <c r="D6" s="4">
-        <v>131</v>
-      </c>
-      <c r="E6" s="4">
         <v>3</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>11</v>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -567,22 +523,16 @@
         <v>44560</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>134</v>
-      </c>
-      <c r="D7" s="4">
-        <v>133</v>
-      </c>
-      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>11</v>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -593,19 +543,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="4">
-        <v>119</v>
-      </c>
-      <c r="D8" s="4">
-        <v>117</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -613,22 +557,16 @@
         <v>44565</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>134</v>
-      </c>
-      <c r="D9" s="4">
-        <v>129</v>
-      </c>
-      <c r="E9" s="4">
         <v>5</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>11</v>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -636,22 +574,16 @@
         <v>44566</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4">
-        <v>134</v>
-      </c>
-      <c r="D10" s="4">
-        <v>132</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -662,12 +594,6 @@
         <v>2</v>
       </c>
       <c r="C11" s="4">
-        <v>119</v>
-      </c>
-      <c r="D11" s="4">
-        <v>119</v>
-      </c>
-      <c r="E11" s="4">
         <v>0</v>
       </c>
     </row>
@@ -676,22 +602,16 @@
         <v>44573</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4">
-        <v>151</v>
-      </c>
-      <c r="D12" s="4">
-        <v>149</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Executed Development and production scripts. All pass
</commit_message>
<xml_diff>
--- a/AUW_Combine/Reports_Combine/Report details.xlsx
+++ b/AUW_Combine/Reports_Combine/Report details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11130" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,8 +614,73 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>44575</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>44575</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>44579</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>44579</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>